<commit_message>
Our User Stories update
</commit_message>
<xml_diff>
--- a/OurUserStories_V1.xlsx
+++ b/OurUserStories_V1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikegalligar/Dropbox/_SeattleU/Quater5/4020_ProPratice/Week_02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikegalligar/Desktop/Git/watts_4020/ancient-fog/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,7 +77,7 @@
     <t>Marketing Admin,</t>
   </si>
   <si>
-    <t>optimizie our marketing.</t>
+    <t>optimize our marketing.</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>